<commit_message>
Update usecase um test darauf aufzubauen
</commit_message>
<xml_diff>
--- a/Doku/Use Case Diagramme/2_UI_UseCaseDiagram_Favoriten.xlsx
+++ b/Doku/Use Case Diagramme/2_UI_UseCaseDiagram_Favoriten.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17830"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabia\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabia\Documents\GitHub\AmazonWatcher\Doku\Use Case Diagramme\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="60">
   <si>
     <t>Use Case Name:</t>
   </si>
@@ -189,9 +189,6 @@
   </si>
   <si>
     <t>Secondary Role (optional):</t>
-  </si>
-  <si>
-    <t>&lt;Name&gt;</t>
   </si>
   <si>
     <t>Ia</t>
@@ -248,15 +245,6 @@
     <t>Einen Favoriten hinzufügen</t>
   </si>
   <si>
-    <t>Schnäppchenjäger</t>
-  </si>
-  <si>
-    <t>Linus (Preisbewusster)</t>
-  </si>
-  <si>
-    <t>Ich möchte statt alle Artikelpreisentwicklungen nur "Favoriten" sehen können die mir besonders wichtig sind</t>
-  </si>
-  <si>
     <t>Zur Übersichtlichkeit sollte dem User ermöglicht werden spezifische Artikel besser verfolgen zu können</t>
   </si>
   <si>
@@ -271,44 +259,50 @@
     <t>User drückt den Favoriten-Button</t>
   </si>
   <si>
+    <t>User kann bei der Erstellung einer neuen Artikelpreisbeobachtung auch einen Favoriten-Button auswählen, sodass der neue Eintrag automatisch in der Favoritenliste erstellt wird.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Welche Zusätzliche Funktionen für die Favoriten dazukommen können ist noch unklar. Angedacht waren Push Benachrichtigungen bei bestimmten Preisen und Uhrzeitabhängige Benachrichtigungen </t>
+  </si>
+  <si>
+    <t>Artikelpreise können gefolgt werden und sind auch vom User gespeichert oder werden im Zuge eines neuen Artikel als Favorit gesetzt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User kann vorhandenen Eintrag über den Favoriten-Button (Herz) zu der Favoritenliste hinzufügen </t>
+  </si>
+  <si>
+    <t>Jeder Artikel hat Name Preis und Bild als Übersicht und je nach Größe der Oberfläche werden mehr oder weniger Artikel gleichzeitig angezeigt</t>
+  </si>
+  <si>
+    <t>Stefan Kreuzer</t>
+  </si>
+  <si>
+    <t>Ich möchte statt alle Artikelpreisentwicklungen "Favoriten" sehen am Anfang sehen können die mir besonders wichtig sind</t>
+  </si>
+  <si>
+    <t>Stefan Kreuzer der Schnäppchenjäger</t>
+  </si>
+  <si>
     <t xml:space="preserve">
-Es werden im Hintergrund nun neue Funktionen aktiviert, sodass eine Favoriten-Ansicht erstellt wird auf die der User nun zugreifen kann
+Es werden im Hintergrund nun diese Artikel höher priorisiert, sodass sie zu Beginn der Seite angezeigt werden
 </t>
   </si>
   <si>
-    <t>User kann bei der Erstellung einer neuen Artikelpreisbeobachtung auch einen Favoriten-Button auswählen, sodass der neue Eintrag automatisch in der Favoritenliste erstellt wird.</t>
-  </si>
-  <si>
-    <t>Diese Übersicht zeigt nur die favorisierten Artikel und deren Preise mit optinaler Entwicklung an</t>
+    <t xml:space="preserve">Diese Übersicht zeigt nur die favorisierten Artikel zuerstund deren Preise mit optinaler Entwicklung an </t>
   </si>
   <si>
     <t xml:space="preserve">
-Auch hier wird (wenn noch keine Favoriten vorhanden) eine neue Favoritenliste angelegt. Die Favoritenseite kann nun aufgerufen werden
+Auch hier wird die Priorität des Artikels erhöht. Die Favoriten sind hier auch zu Beginn aufgelistet
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Der User kommt erneut auf die Website, da er nun Favoriten hat werden diese als Startbildschirm angezeigt </t>
-  </si>
-  <si>
-    <t>User sieht im Überblick alle seine Favoriten</t>
-  </si>
-  <si>
-    <t>Im Hintergrund wird als neue Startseite die Favoritenübersicht gesetzt, sodass bei jedem neuen Aufrufen die Favoriten angezeigt werden</t>
-  </si>
-  <si>
-    <t>Favoriten sind auf der Startseite</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Welche Zusätzliche Funktionen für die Favoriten dazukommen können ist noch unklar. Angedacht waren Push Benachrichtigungen bei bestimmten Preisen und Uhrzeitabhängige Benachrichtigungen </t>
-  </si>
-  <si>
-    <t>Artikelpreise können gefolgt werden und sind auch vom User gespeichert oder werden im Zuge eines neuen Artikel als Favorit gesetzt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User kann vorhandenen Eintrag über den Favoriten-Button (Herz) zu der Favoritenliste hinzufügen </t>
-  </si>
-  <si>
-    <t>Jeder Artikel hat Name Preis und Bild als Übersicht und je nach Größe der Oberfläche werden mehr oder weniger Artikel gleichzeitig angezeigt</t>
+    <t>Die Übersicht zeigt nur die favorisierten Artikel zuerst und deren Preise mit optinaler Entwicklung an</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Der User kommt erneut auf die Website, da er nun Favoriten hat werden diese als erstes angezeigt </t>
+  </si>
+  <si>
+    <t>User sieht im Überblick alle seine Favoriten zuerst</t>
   </si>
 </sst>
 </file>
@@ -682,6 +676,15 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -714,15 +717,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1202,12 +1196,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="de-DE" sz="1000">
-                <a:latin typeface="BentonSans Regular" panose="02000503000000020004" pitchFamily="2" charset="0"/>
-              </a:rPr>
-              <a:t>&lt;Reason for Iteration&gt;</a:t>
-            </a:r>
+            <a:endParaRPr lang="de-DE" sz="1000">
+              <a:latin typeface="BentonSans Regular" panose="02000503000000020004" pitchFamily="2" charset="0"/>
+            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1362,62 +1353,6 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>314325</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>352425</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="49" name="Straight Arrow Connector 48">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000031000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5486400" y="10325100"/>
-          <a:ext cx="1057275" cy="866775"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="25400">
-          <a:solidFill>
-            <a:srgbClr val="996792"/>
-          </a:solidFill>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
@@ -1596,6 +1531,62 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1155249</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>44223</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2371725</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Grafik 18" descr="C:\Users\fabia\Downloads\profile-max-mustermann.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B4AAEC1-37E5-4CAF-B93C-AB96DF1167C7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="17456" t="1509" r="16515" b="16238"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2545899" y="4259036"/>
+          <a:ext cx="1216476" cy="1046389"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{53640926-AAD7-44D8-BBD7-CCE9431645EC}">
+            <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2837,8 +2828,8 @@
   </sheetPr>
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="40" zoomScalePageLayoutView="20" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" zoomScaleSheetLayoutView="40" zoomScalePageLayoutView="20" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="12.75"/>
@@ -2857,7 +2848,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="17" customFormat="1" ht="59.65">
       <c r="A1" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C1" s="18"/>
       <c r="D1" s="18"/>
@@ -2869,17 +2860,17 @@
       <c r="J1" s="19"/>
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1">
-      <c r="A2" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
+      <c r="A2" s="46" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
       <c r="J2" s="18"/>
     </row>
     <row r="3" spans="1:10" ht="20.100000000000001" customHeight="1">
@@ -2896,34 +2887,34 @@
     </row>
     <row r="4" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A4" s="3"/>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="D4" s="52">
+      <c r="C4" s="39"/>
+      <c r="D4" s="40">
         <v>1</v>
       </c>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="52"/>
-      <c r="I4" s="52"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
       <c r="J4" s="4"/>
     </row>
     <row r="5" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A5" s="3"/>
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="51"/>
-      <c r="D5" s="50" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50"/>
-      <c r="H5" s="50"/>
-      <c r="I5" s="50"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
       <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:10" ht="9.9499999999999993" customHeight="1">
@@ -2940,98 +2931,96 @@
     </row>
     <row r="7" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A7" s="3"/>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="51"/>
-      <c r="D7" s="50" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="50"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="50"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
       <c r="J7" s="4"/>
     </row>
     <row r="8" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A8" s="3"/>
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="51"/>
-      <c r="D8" s="50" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8" s="50"/>
-      <c r="F8" s="50"/>
-      <c r="G8" s="50"/>
-      <c r="H8" s="50"/>
-      <c r="I8" s="50"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
       <c r="J8" s="4"/>
     </row>
     <row r="9" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A9" s="3"/>
-      <c r="B9" s="51" t="s">
+      <c r="B9" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="51"/>
-      <c r="D9" s="50" t="s">
-        <v>45</v>
-      </c>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="50"/>
-      <c r="H9" s="50"/>
-      <c r="I9" s="50"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
       <c r="J9" s="4"/>
     </row>
     <row r="10" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A10" s="3"/>
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="51"/>
-      <c r="D10" s="50" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10" s="50"/>
-      <c r="F10" s="50"/>
-      <c r="G10" s="50"/>
-      <c r="H10" s="50"/>
-      <c r="I10" s="50"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
       <c r="J10" s="4"/>
     </row>
     <row r="11" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A11" s="3"/>
-      <c r="B11" s="51" t="s">
+      <c r="B11" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="51"/>
-      <c r="D11" s="50" t="s">
-        <v>59</v>
-      </c>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="50"/>
-      <c r="H11" s="50"/>
-      <c r="I11" s="50"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="41"/>
       <c r="J11" s="4"/>
     </row>
     <row r="12" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A12" s="3"/>
-      <c r="B12" s="51" t="s">
+      <c r="B12" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="51"/>
-      <c r="D12" s="50" t="s">
-        <v>47</v>
-      </c>
-      <c r="E12" s="50"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="50"/>
-      <c r="H12" s="50"/>
-      <c r="I12" s="50"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="41"/>
       <c r="J12" s="4"/>
     </row>
     <row r="13" spans="1:10">
@@ -3048,20 +3037,20 @@
     </row>
     <row r="14" spans="1:10" s="15" customFormat="1" ht="36" customHeight="1">
       <c r="A14" s="13"/>
-      <c r="B14" s="44" t="s">
+      <c r="B14" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="48" t="s">
+      <c r="C14" s="48"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="49"/>
-      <c r="G14" s="46" t="s">
+      <c r="F14" s="52"/>
+      <c r="G14" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="H14" s="47"/>
-      <c r="I14" s="47"/>
+      <c r="H14" s="50"/>
+      <c r="I14" s="50"/>
       <c r="J14" s="14"/>
     </row>
     <row r="15" spans="1:10" ht="20.100000000000001" customHeight="1">
@@ -3150,16 +3139,16 @@
     </row>
     <row r="22" spans="1:10" ht="15" customHeight="1">
       <c r="A22" s="12"/>
-      <c r="B22" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="40"/>
-      <c r="D22" s="40"/>
+      <c r="B22" s="43" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="43"/>
+      <c r="D22" s="43"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="39"/>
+      <c r="G22" s="42"/>
+      <c r="H22" s="42"/>
+      <c r="I22" s="42"/>
       <c r="J22" s="4"/>
     </row>
     <row r="23" spans="1:10" ht="15" customHeight="1" thickBot="1">
@@ -3180,17 +3169,17 @@
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="30">
         <v>1</v>
       </c>
       <c r="H24" s="29" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I24" s="29" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="J24" s="4"/>
     </row>
@@ -3200,13 +3189,13 @@
         <v>2</v>
       </c>
       <c r="C25" s="28" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="D25" s="27" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E25" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="7"/>
@@ -3218,7 +3207,7 @@
       <c r="A26" s="12"/>
       <c r="B26" s="6"/>
       <c r="C26" s="33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="3"/>
@@ -3227,10 +3216,10 @@
         <v>3</v>
       </c>
       <c r="H26" s="29" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="I26" s="29" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="J26" s="4"/>
     </row>
@@ -3240,10 +3229,10 @@
         <v>4</v>
       </c>
       <c r="C27" s="28" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D27" s="27" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
@@ -3263,10 +3252,10 @@
         <v>5</v>
       </c>
       <c r="H28" s="29" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="I28" s="29" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="J28" s="4"/>
     </row>
@@ -3274,10 +3263,10 @@
       <c r="A29" s="31"/>
       <c r="B29" s="26"/>
       <c r="C29" s="28" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D29" s="27" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
@@ -3286,7 +3275,7 @@
       <c r="I29" s="25"/>
       <c r="J29" s="4"/>
     </row>
-    <row r="30" spans="1:10" ht="39" thickTop="1" thickBot="1">
+    <row r="30" spans="1:10" ht="21" thickTop="1" thickBot="1">
       <c r="A30" s="12"/>
       <c r="B30" s="6"/>
       <c r="C30" s="33"/>
@@ -3294,12 +3283,8 @@
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
       <c r="G30" s="30"/>
-      <c r="H30" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="I30" s="29" t="s">
-        <v>57</v>
-      </c>
+      <c r="H30" s="29"/>
+      <c r="I30" s="29"/>
       <c r="J30" s="4"/>
     </row>
     <row r="31" spans="1:10" ht="15" customHeight="1" thickTop="1">
@@ -3340,30 +3325,30 @@
     </row>
     <row r="34" spans="1:10" ht="15" customHeight="1">
       <c r="A34" s="5"/>
-      <c r="B34" s="41" t="s">
+      <c r="B34" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="C34" s="41"/>
-      <c r="D34" s="41"/>
-      <c r="E34" s="41"/>
-      <c r="F34" s="41"/>
-      <c r="G34" s="41"/>
-      <c r="H34" s="41"/>
-      <c r="I34" s="41"/>
+      <c r="C34" s="44"/>
+      <c r="D34" s="44"/>
+      <c r="E34" s="44"/>
+      <c r="F34" s="44"/>
+      <c r="G34" s="44"/>
+      <c r="H34" s="44"/>
+      <c r="I34" s="44"/>
       <c r="J34" s="8"/>
     </row>
     <row r="35" spans="1:10" ht="89.25" customHeight="1">
       <c r="A35" s="5"/>
-      <c r="B35" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="C35" s="42"/>
-      <c r="D35" s="42"/>
-      <c r="E35" s="42"/>
-      <c r="F35" s="42"/>
-      <c r="G35" s="42"/>
-      <c r="H35" s="42"/>
-      <c r="I35" s="42"/>
+      <c r="B35" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35" s="45"/>
+      <c r="D35" s="45"/>
+      <c r="E35" s="45"/>
+      <c r="F35" s="45"/>
+      <c r="G35" s="45"/>
+      <c r="H35" s="45"/>
+      <c r="I35" s="45"/>
       <c r="J35" s="8"/>
     </row>
     <row r="36" spans="1:10">
@@ -3428,14 +3413,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D4:I4"/>
-    <mergeCell ref="D5:I5"/>
-    <mergeCell ref="D7:I7"/>
-    <mergeCell ref="D8:I8"/>
-    <mergeCell ref="D9:I9"/>
-    <mergeCell ref="D10:I10"/>
     <mergeCell ref="G22:I22"/>
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="B34:I34"/>
@@ -3452,6 +3429,14 @@
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D4:I4"/>
+    <mergeCell ref="D5:I5"/>
+    <mergeCell ref="D7:I7"/>
+    <mergeCell ref="D8:I8"/>
+    <mergeCell ref="D9:I9"/>
+    <mergeCell ref="D10:I10"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2:I2" r:id="rId1" display="Click here to find more information about Use Case Diagram and Methodology"/>
@@ -3490,7 +3475,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="17" customFormat="1" ht="59.65">
       <c r="A1" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C1" s="18"/>
       <c r="D1" s="18"/>
@@ -3502,17 +3487,17 @@
       <c r="J1" s="19"/>
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1">
-      <c r="A2" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
+      <c r="A2" s="46" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
       <c r="J2" s="18"/>
     </row>
     <row r="3" spans="1:10" ht="20.100000000000001" customHeight="1">
@@ -3529,34 +3514,34 @@
     </row>
     <row r="4" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A4" s="3"/>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="D4" s="52" t="s">
+      <c r="C4" s="39"/>
+      <c r="D4" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="52"/>
-      <c r="I4" s="52"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
       <c r="J4" s="4"/>
     </row>
     <row r="5" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A5" s="3"/>
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="51"/>
-      <c r="D5" s="50" t="s">
+      <c r="C5" s="39"/>
+      <c r="D5" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50"/>
-      <c r="H5" s="50"/>
-      <c r="I5" s="50"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
       <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:10" ht="9.9499999999999993" customHeight="1">
@@ -3573,96 +3558,96 @@
     </row>
     <row r="7" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A7" s="3"/>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="51"/>
-      <c r="D7" s="50" t="s">
+      <c r="C7" s="39"/>
+      <c r="D7" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="50"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="50"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
       <c r="J7" s="4"/>
     </row>
     <row r="8" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A8" s="3"/>
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="51"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="50"/>
-      <c r="G8" s="50"/>
-      <c r="H8" s="50"/>
-      <c r="I8" s="50"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
       <c r="J8" s="4"/>
     </row>
     <row r="9" spans="1:10" ht="32.25" customHeight="1">
       <c r="A9" s="3"/>
-      <c r="B9" s="51" t="s">
+      <c r="B9" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="51"/>
-      <c r="D9" s="50" t="s">
+      <c r="C9" s="39"/>
+      <c r="D9" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="50"/>
-      <c r="H9" s="50"/>
-      <c r="I9" s="50"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
       <c r="J9" s="4"/>
     </row>
     <row r="10" spans="1:10" ht="45.75" customHeight="1">
       <c r="A10" s="3"/>
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="51"/>
-      <c r="D10" s="50" t="s">
+      <c r="C10" s="39"/>
+      <c r="D10" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="50"/>
-      <c r="F10" s="50"/>
-      <c r="G10" s="50"/>
-      <c r="H10" s="50"/>
-      <c r="I10" s="50"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
       <c r="J10" s="4"/>
     </row>
     <row r="11" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A11" s="3"/>
-      <c r="B11" s="51" t="s">
+      <c r="B11" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="51"/>
-      <c r="D11" s="50" t="s">
+      <c r="C11" s="39"/>
+      <c r="D11" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="50"/>
-      <c r="H11" s="50"/>
-      <c r="I11" s="50"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="41"/>
       <c r="J11" s="4"/>
     </row>
     <row r="12" spans="1:10" ht="33.75" customHeight="1">
       <c r="A12" s="3"/>
-      <c r="B12" s="51" t="s">
+      <c r="B12" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="51"/>
-      <c r="D12" s="50" t="s">
+      <c r="C12" s="39"/>
+      <c r="D12" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="50"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="50"/>
-      <c r="H12" s="50"/>
-      <c r="I12" s="50"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="41"/>
       <c r="J12" s="4"/>
     </row>
     <row r="13" spans="1:10">
@@ -3679,20 +3664,20 @@
     </row>
     <row r="14" spans="1:10" s="15" customFormat="1" ht="36" customHeight="1">
       <c r="A14" s="13"/>
-      <c r="B14" s="44" t="s">
+      <c r="B14" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="48" t="s">
+      <c r="C14" s="48"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="49"/>
-      <c r="G14" s="46" t="s">
+      <c r="F14" s="52"/>
+      <c r="G14" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="H14" s="47"/>
-      <c r="I14" s="47"/>
+      <c r="H14" s="50"/>
+      <c r="I14" s="50"/>
       <c r="J14" s="14"/>
     </row>
     <row r="15" spans="1:10" ht="20.100000000000001" customHeight="1">
@@ -3715,7 +3700,7 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H16" s="25"/>
       <c r="I16" s="25"/>
@@ -3784,24 +3769,24 @@
     <row r="22" spans="1:10" ht="15" customHeight="1">
       <c r="A22" s="12"/>
       <c r="B22" s="6"/>
-      <c r="C22" s="40"/>
-      <c r="D22" s="40"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="43"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
-      <c r="G22" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="H22" s="39"/>
-      <c r="I22" s="39"/>
+      <c r="G22" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="H22" s="42"/>
+      <c r="I22" s="42"/>
       <c r="J22" s="4"/>
     </row>
     <row r="23" spans="1:10" ht="15" customHeight="1" thickBot="1">
       <c r="A23" s="12"/>
-      <c r="B23" s="40" t="s">
+      <c r="B23" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="25"/>
@@ -3815,10 +3800,10 @@
       <c r="C24" s="24"/>
       <c r="D24" s="6"/>
       <c r="E24" s="36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F24" s="38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G24" s="30">
         <v>1</v>
@@ -3831,7 +3816,7 @@
     </row>
     <row r="25" spans="1:10" ht="21" thickTop="1" thickBot="1">
       <c r="A25" s="37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B25" s="26">
         <v>2</v>
@@ -3993,28 +3978,28 @@
     </row>
     <row r="35" spans="1:10" ht="15" customHeight="1">
       <c r="A35" s="5"/>
-      <c r="B35" s="41" t="s">
+      <c r="B35" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="C35" s="41"/>
-      <c r="D35" s="41"/>
-      <c r="E35" s="41"/>
-      <c r="F35" s="41"/>
-      <c r="G35" s="41"/>
-      <c r="H35" s="41"/>
-      <c r="I35" s="41"/>
+      <c r="C35" s="44"/>
+      <c r="D35" s="44"/>
+      <c r="E35" s="44"/>
+      <c r="F35" s="44"/>
+      <c r="G35" s="44"/>
+      <c r="H35" s="44"/>
+      <c r="I35" s="44"/>
       <c r="J35" s="8"/>
     </row>
     <row r="36" spans="1:10" ht="89.25" customHeight="1">
       <c r="A36" s="5"/>
-      <c r="B36" s="42"/>
-      <c r="C36" s="42"/>
-      <c r="D36" s="42"/>
-      <c r="E36" s="42"/>
-      <c r="F36" s="42"/>
-      <c r="G36" s="42"/>
-      <c r="H36" s="42"/>
-      <c r="I36" s="42"/>
+      <c r="B36" s="45"/>
+      <c r="C36" s="45"/>
+      <c r="D36" s="45"/>
+      <c r="E36" s="45"/>
+      <c r="F36" s="45"/>
+      <c r="G36" s="45"/>
+      <c r="H36" s="45"/>
+      <c r="I36" s="45"/>
       <c r="J36" s="8"/>
     </row>
     <row r="37" spans="1:10">
@@ -4079,15 +4064,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B35:I35"/>
-    <mergeCell ref="B36:I36"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:I11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:I12"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:I14"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="D7:I7"/>
     <mergeCell ref="G22:I22"/>
@@ -4104,6 +4080,15 @@
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="D10:I10"/>
     <mergeCell ref="C22:D22"/>
+    <mergeCell ref="B35:I35"/>
+    <mergeCell ref="B36:I36"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:I11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:I12"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:I14"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2:I2" r:id="rId1" display="Click here to find more information about Use Case Diagram and Methodology"/>

</xml_diff>